<commit_message>
Bug fix: remove olhc data carryover
</commit_message>
<xml_diff>
--- a/src/dataout/18mpip.xlsx
+++ b/src/dataout/18mpip.xlsx
@@ -869,18 +869,6 @@
       <c r="A5" s="2">
         <v>43105</v>
       </c>
-      <c r="B5">
-        <v>1.35439</v>
-      </c>
-      <c r="C5">
-        <v>1.35822</v>
-      </c>
-      <c r="D5">
-        <v>1.35232</v>
-      </c>
-      <c r="E5">
-        <v>1.35659</v>
-      </c>
       <c r="F5">
         <v>1.35622</v>
       </c>
@@ -1272,18 +1260,6 @@
       <c r="A10" s="2">
         <v>43112</v>
       </c>
-      <c r="B10">
-        <v>1.35354</v>
-      </c>
-      <c r="C10">
-        <v>1.3744</v>
-      </c>
-      <c r="D10">
-        <v>1.35346</v>
-      </c>
-      <c r="E10">
-        <v>1.37275</v>
-      </c>
       <c r="F10">
         <v>1.36733</v>
       </c>
@@ -1657,18 +1633,6 @@
       <c r="A15" s="2">
         <v>43119</v>
       </c>
-      <c r="B15">
-        <v>1.38905</v>
-      </c>
-      <c r="C15">
-        <v>1.39452</v>
-      </c>
-      <c r="D15">
-        <v>1.38384</v>
-      </c>
-      <c r="E15">
-        <v>1.38468</v>
-      </c>
       <c r="F15">
         <v>1.3864</v>
       </c>
@@ -2042,18 +2006,6 @@
       <c r="A20" s="2">
         <v>43126</v>
       </c>
-      <c r="B20">
-        <v>1.41312</v>
-      </c>
-      <c r="C20">
-        <v>1.42866</v>
-      </c>
-      <c r="D20">
-        <v>1.41078</v>
-      </c>
-      <c r="E20">
-        <v>1.41552</v>
-      </c>
       <c r="F20">
         <v>1.41631</v>
       </c>
@@ -2427,18 +2379,6 @@
       <c r="A25" s="2">
         <v>43133</v>
       </c>
-      <c r="B25">
-        <v>1.42507</v>
-      </c>
-      <c r="C25">
-        <v>1.42782</v>
-      </c>
-      <c r="D25">
-        <v>1.41014</v>
-      </c>
-      <c r="E25">
-        <v>1.41216</v>
-      </c>
       <c r="F25">
         <v>1.41291</v>
       </c>
@@ -2818,18 +2758,6 @@
       <c r="A30" s="2">
         <v>43140</v>
       </c>
-      <c r="B30">
-        <v>1.39096</v>
-      </c>
-      <c r="C30">
-        <v>1.39871</v>
-      </c>
-      <c r="D30">
-        <v>1.37646</v>
-      </c>
-      <c r="E30">
-        <v>1.38248</v>
-      </c>
       <c r="F30">
         <v>1.3801</v>
       </c>
@@ -3209,18 +3137,6 @@
       <c r="A35" s="2">
         <v>43147</v>
       </c>
-      <c r="B35">
-        <v>1.40945</v>
-      </c>
-      <c r="C35">
-        <v>1.41448</v>
-      </c>
-      <c r="D35">
-        <v>1.39966</v>
-      </c>
-      <c r="E35">
-        <v>1.40297</v>
-      </c>
       <c r="F35">
         <v>1.40462</v>
       </c>
@@ -3606,18 +3522,6 @@
       <c r="A40" s="2">
         <v>43154</v>
       </c>
-      <c r="B40">
-        <v>1.39507</v>
-      </c>
-      <c r="C40">
-        <v>1.40053</v>
-      </c>
-      <c r="D40">
-        <v>1.39042</v>
-      </c>
-      <c r="E40">
-        <v>1.39678</v>
-      </c>
       <c r="F40">
         <v>1.39908</v>
       </c>
@@ -3991,18 +3895,6 @@
       <c r="A45" s="2">
         <v>43161</v>
       </c>
-      <c r="B45">
-        <v>1.37711</v>
-      </c>
-      <c r="C45">
-        <v>1.38167</v>
-      </c>
-      <c r="D45">
-        <v>1.37555</v>
-      </c>
-      <c r="E45">
-        <v>1.37993</v>
-      </c>
       <c r="F45">
         <v>1.37769</v>
       </c>
@@ -4382,18 +4274,6 @@
       <c r="A50" s="2">
         <v>43168</v>
       </c>
-      <c r="B50">
-        <v>1.3807</v>
-      </c>
-      <c r="C50">
-        <v>1.3889</v>
-      </c>
-      <c r="D50">
-        <v>1.3788</v>
-      </c>
-      <c r="E50">
-        <v>1.38497</v>
-      </c>
       <c r="F50">
         <v>1.38778</v>
       </c>
@@ -4767,18 +4647,6 @@
       <c r="A55" s="2">
         <v>43175</v>
       </c>
-      <c r="B55">
-        <v>1.39356</v>
-      </c>
-      <c r="C55">
-        <v>1.39806</v>
-      </c>
-      <c r="D55">
-        <v>1.38896</v>
-      </c>
-      <c r="E55">
-        <v>1.3937</v>
-      </c>
       <c r="F55">
         <v>1.39282</v>
       </c>
@@ -5152,18 +5020,6 @@
       <c r="A60" s="2">
         <v>43182</v>
       </c>
-      <c r="B60">
-        <v>1.40948</v>
-      </c>
-      <c r="C60">
-        <v>1.41718</v>
-      </c>
-      <c r="D60">
-        <v>1.4085</v>
-      </c>
-      <c r="E60">
-        <v>1.41295</v>
-      </c>
       <c r="F60">
         <v>1.41601</v>
       </c>
@@ -5537,18 +5393,6 @@
       <c r="A65" s="2">
         <v>43189</v>
       </c>
-      <c r="B65">
-        <v>1.40175</v>
-      </c>
-      <c r="C65">
-        <v>1.40598</v>
-      </c>
-      <c r="D65">
-        <v>1.40125</v>
-      </c>
-      <c r="E65">
-        <v>1.40183</v>
-      </c>
       <c r="F65">
         <v>1.40365</v>
       </c>
@@ -5919,18 +5763,6 @@
       <c r="A70" s="2">
         <v>43196</v>
       </c>
-      <c r="B70">
-        <v>1.40005</v>
-      </c>
-      <c r="C70">
-        <v>1.41054</v>
-      </c>
-      <c r="D70">
-        <v>1.39831</v>
-      </c>
-      <c r="E70">
-        <v>1.4088</v>
-      </c>
       <c r="F70">
         <v>1.40935</v>
       </c>
@@ -6304,18 +6136,6 @@
       <c r="A75" s="2">
         <v>43203</v>
       </c>
-      <c r="B75">
-        <v>1.42271</v>
-      </c>
-      <c r="C75">
-        <v>1.42964</v>
-      </c>
-      <c r="D75">
-        <v>1.42208</v>
-      </c>
-      <c r="E75">
-        <v>1.42379</v>
-      </c>
       <c r="F75">
         <v>1.42528</v>
       </c>
@@ -6689,18 +6509,6 @@
       <c r="A80" s="2">
         <v>43210</v>
       </c>
-      <c r="B80">
-        <v>1.40824</v>
-      </c>
-      <c r="C80">
-        <v>1.40909</v>
-      </c>
-      <c r="D80">
-        <v>1.40005</v>
-      </c>
-      <c r="E80">
-        <v>1.40005</v>
-      </c>
       <c r="F80">
         <v>1.40203</v>
       </c>
@@ -7080,18 +6888,6 @@
       <c r="A85" s="2">
         <v>43217</v>
       </c>
-      <c r="B85">
-        <v>1.39118</v>
-      </c>
-      <c r="C85">
-        <v>1.39344</v>
-      </c>
-      <c r="D85">
-        <v>1.37472</v>
-      </c>
-      <c r="E85">
-        <v>1.37748</v>
-      </c>
       <c r="F85">
         <v>1.37781</v>
       </c>
@@ -7471,18 +7267,6 @@
       <c r="A90" s="2">
         <v>43224</v>
       </c>
-      <c r="B90">
-        <v>1.35737</v>
-      </c>
-      <c r="C90">
-        <v>1.3586</v>
-      </c>
-      <c r="D90">
-        <v>1.34863</v>
-      </c>
-      <c r="E90">
-        <v>1.35249</v>
-      </c>
       <c r="F90">
         <v>1.35118</v>
       </c>
@@ -7856,18 +7640,6 @@
       <c r="A95" s="2">
         <v>43231</v>
       </c>
-      <c r="B95">
-        <v>1.35148</v>
-      </c>
-      <c r="C95">
-        <v>1.35956</v>
-      </c>
-      <c r="D95">
-        <v>1.3502</v>
-      </c>
-      <c r="E95">
-        <v>1.35393</v>
-      </c>
       <c r="F95">
         <v>1.35671</v>
       </c>
@@ -8241,18 +8013,6 @@
       <c r="A100" s="2">
         <v>43238</v>
       </c>
-      <c r="B100">
-        <v>1.35148</v>
-      </c>
-      <c r="C100">
-        <v>1.35281</v>
-      </c>
-      <c r="D100">
-        <v>1.34551</v>
-      </c>
-      <c r="E100">
-        <v>1.34692</v>
-      </c>
       <c r="F100">
         <v>1.34704</v>
       </c>
@@ -8626,18 +8386,6 @@
       <c r="A105" s="2">
         <v>43245</v>
       </c>
-      <c r="B105">
-        <v>1.33772</v>
-      </c>
-      <c r="C105">
-        <v>1.33881</v>
-      </c>
-      <c r="D105">
-        <v>1.32941</v>
-      </c>
-      <c r="E105">
-        <v>1.3297</v>
-      </c>
       <c r="F105">
         <v>1.33136</v>
       </c>
@@ -9017,18 +8765,6 @@
       <c r="A110" s="2">
         <v>43252</v>
       </c>
-      <c r="B110">
-        <v>1.32936</v>
-      </c>
-      <c r="C110">
-        <v>1.33618</v>
-      </c>
-      <c r="D110">
-        <v>1.32539</v>
-      </c>
-      <c r="E110">
-        <v>1.33491</v>
-      </c>
       <c r="F110">
         <v>1.33238</v>
       </c>
@@ -9408,18 +9144,6 @@
       <c r="A115" s="2">
         <v>43259</v>
       </c>
-      <c r="B115">
-        <v>1.34209</v>
-      </c>
-      <c r="C115">
-        <v>1.34391</v>
-      </c>
-      <c r="D115">
-        <v>1.33547</v>
-      </c>
-      <c r="E115">
-        <v>1.34074</v>
-      </c>
       <c r="F115">
         <v>1.33881</v>
       </c>
@@ -9799,18 +9523,6 @@
       <c r="A120" s="2">
         <v>43266</v>
       </c>
-      <c r="B120">
-        <v>1.32599</v>
-      </c>
-      <c r="C120">
-        <v>1.32983</v>
-      </c>
-      <c r="D120">
-        <v>1.32113</v>
-      </c>
-      <c r="E120">
-        <v>1.32812</v>
-      </c>
       <c r="F120">
         <v>1.32755</v>
       </c>
@@ -10184,18 +9896,6 @@
       <c r="A125" s="2">
         <v>43273</v>
       </c>
-      <c r="B125">
-        <v>1.324</v>
-      </c>
-      <c r="C125">
-        <v>1.33151</v>
-      </c>
-      <c r="D125">
-        <v>1.32297</v>
-      </c>
-      <c r="E125">
-        <v>1.32626</v>
-      </c>
       <c r="F125">
         <v>1.32552</v>
       </c>
@@ -10581,18 +10281,6 @@
       <c r="A130" s="2">
         <v>43280</v>
       </c>
-      <c r="B130">
-        <v>1.30759</v>
-      </c>
-      <c r="C130">
-        <v>1.32134</v>
-      </c>
-      <c r="D130">
-        <v>1.30674</v>
-      </c>
-      <c r="E130">
-        <v>1.32066</v>
-      </c>
       <c r="F130">
         <v>1.31729</v>
       </c>
@@ -10966,18 +10654,6 @@
       <c r="A135" s="2">
         <v>43287</v>
       </c>
-      <c r="B135">
-        <v>1.32094</v>
-      </c>
-      <c r="C135">
-        <v>1.32901</v>
-      </c>
-      <c r="D135">
-        <v>1.32034</v>
-      </c>
-      <c r="E135">
-        <v>1.32824</v>
-      </c>
       <c r="F135">
         <v>1.32713</v>
       </c>
@@ -11357,18 +11033,6 @@
       <c r="A140" s="2">
         <v>43294</v>
       </c>
-      <c r="B140">
-        <v>1.32027</v>
-      </c>
-      <c r="C140">
-        <v>1.32384</v>
-      </c>
-      <c r="D140">
-        <v>1.31026</v>
-      </c>
-      <c r="E140">
-        <v>1.32373</v>
-      </c>
       <c r="F140">
         <v>1.31828</v>
       </c>
@@ -11742,18 +11406,6 @@
       <c r="A145" s="2">
         <v>43301</v>
       </c>
-      <c r="B145">
-        <v>1.30136</v>
-      </c>
-      <c r="C145">
-        <v>1.31398</v>
-      </c>
-      <c r="D145">
-        <v>1.2995</v>
-      </c>
-      <c r="E145">
-        <v>1.31296</v>
-      </c>
       <c r="F145">
         <v>1.31062</v>
       </c>
@@ -12133,18 +11785,6 @@
       <c r="A150" s="2">
         <v>43308</v>
       </c>
-      <c r="B150">
-        <v>1.31054</v>
-      </c>
-      <c r="C150">
-        <v>1.3131</v>
-      </c>
-      <c r="D150">
-        <v>1.30828</v>
-      </c>
-      <c r="E150">
-        <v>1.31016</v>
-      </c>
       <c r="F150">
         <v>1.31185</v>
       </c>
@@ -12518,18 +12158,6 @@
       <c r="A155" s="2">
         <v>43315</v>
       </c>
-      <c r="B155">
-        <v>1.30116</v>
-      </c>
-      <c r="C155">
-        <v>1.30432</v>
-      </c>
-      <c r="D155">
-        <v>1.29754</v>
-      </c>
-      <c r="E155">
-        <v>1.3002</v>
-      </c>
       <c r="F155">
         <v>1.3004</v>
       </c>
@@ -12909,18 +12537,6 @@
       <c r="A160" s="2">
         <v>43322</v>
       </c>
-      <c r="B160">
-        <v>1.28238</v>
-      </c>
-      <c r="C160">
-        <v>1.28366</v>
-      </c>
-      <c r="D160">
-        <v>1.27226</v>
-      </c>
-      <c r="E160">
-        <v>1.2771</v>
-      </c>
       <c r="F160">
         <v>1.27628</v>
       </c>
@@ -13294,18 +12910,6 @@
       <c r="A165" s="2">
         <v>43329</v>
       </c>
-      <c r="B165">
-        <v>1.27094</v>
-      </c>
-      <c r="C165">
-        <v>1.27528</v>
-      </c>
-      <c r="D165">
-        <v>1.26979</v>
-      </c>
-      <c r="E165">
-        <v>1.27508</v>
-      </c>
       <c r="F165">
         <v>1.27286</v>
       </c>
@@ -13679,18 +13283,6 @@
       <c r="A170" s="2">
         <v>43336</v>
       </c>
-      <c r="B170">
-        <v>1.28095</v>
-      </c>
-      <c r="C170">
-        <v>1.28811</v>
-      </c>
-      <c r="D170">
-        <v>1.27993</v>
-      </c>
-      <c r="E170">
-        <v>1.28488</v>
-      </c>
       <c r="F170">
         <v>1.28557</v>
       </c>
@@ -14064,18 +13656,6 @@
       <c r="A175" s="2">
         <v>43343</v>
       </c>
-      <c r="B175">
-        <v>1.30055</v>
-      </c>
-      <c r="C175">
-        <v>1.30286</v>
-      </c>
-      <c r="D175">
-        <v>1.29454</v>
-      </c>
-      <c r="E175">
-        <v>1.29567</v>
-      </c>
       <c r="F175">
         <v>1.29836</v>
       </c>
@@ -14449,18 +14029,6 @@
       <c r="A180" s="2">
         <v>43350</v>
       </c>
-      <c r="B180">
-        <v>1.29257</v>
-      </c>
-      <c r="C180">
-        <v>1.30284</v>
-      </c>
-      <c r="D180">
-        <v>1.29082</v>
-      </c>
-      <c r="E180">
-        <v>1.29159</v>
-      </c>
       <c r="F180">
         <v>1.29648</v>
       </c>
@@ -14840,18 +14408,6 @@
       <c r="A185" s="2">
         <v>43357</v>
       </c>
-      <c r="B185">
-        <v>1.31058</v>
-      </c>
-      <c r="C185">
-        <v>1.31429</v>
-      </c>
-      <c r="D185">
-        <v>1.30566</v>
-      </c>
-      <c r="E185">
-        <v>1.30689</v>
-      </c>
       <c r="F185">
         <v>1.30782</v>
       </c>
@@ -15237,18 +14793,6 @@
       <c r="A190" s="2">
         <v>43364</v>
       </c>
-      <c r="B190">
-        <v>1.32629</v>
-      </c>
-      <c r="C190">
-        <v>1.32766</v>
-      </c>
-      <c r="D190">
-        <v>1.30548</v>
-      </c>
-      <c r="E190">
-        <v>1.30831</v>
-      </c>
       <c r="F190">
         <v>1.30835</v>
       </c>
@@ -15622,18 +15166,6 @@
       <c r="A195" s="2">
         <v>43371</v>
       </c>
-      <c r="B195">
-        <v>1.30741</v>
-      </c>
-      <c r="C195">
-        <v>1.30901</v>
-      </c>
-      <c r="D195">
-        <v>1.30005</v>
-      </c>
-      <c r="E195">
-        <v>1.30282</v>
-      </c>
       <c r="F195">
         <v>1.30072</v>
       </c>
@@ -16007,18 +15539,6 @@
       <c r="A200" s="2">
         <v>43378</v>
       </c>
-      <c r="B200">
-        <v>1.3021</v>
-      </c>
-      <c r="C200">
-        <v>1.31226</v>
-      </c>
-      <c r="D200">
-        <v>1.30034</v>
-      </c>
-      <c r="E200">
-        <v>1.31148</v>
-      </c>
       <c r="F200">
         <v>1.3077</v>
       </c>
@@ -16392,18 +15912,6 @@
       <c r="A205" s="2">
         <v>43385</v>
       </c>
-      <c r="B205">
-        <v>1.3226</v>
-      </c>
-      <c r="C205">
-        <v>1.32577</v>
-      </c>
-      <c r="D205">
-        <v>1.31469</v>
-      </c>
-      <c r="E205">
-        <v>1.31525</v>
-      </c>
       <c r="F205">
         <v>1.31847</v>
       </c>
@@ -16783,18 +16291,6 @@
       <c r="A210" s="2">
         <v>43392</v>
       </c>
-      <c r="B210">
-        <v>1.30174</v>
-      </c>
-      <c r="C210">
-        <v>1.31042</v>
-      </c>
-      <c r="D210">
-        <v>1.30113</v>
-      </c>
-      <c r="E210">
-        <v>1.30652</v>
-      </c>
       <c r="F210">
         <v>1.30471</v>
       </c>
@@ -17174,18 +16670,6 @@
       <c r="A215" s="2">
         <v>43399</v>
       </c>
-      <c r="B215">
-        <v>1.2815</v>
-      </c>
-      <c r="C215">
-        <v>1.28414</v>
-      </c>
-      <c r="D215">
-        <v>1.27772</v>
-      </c>
-      <c r="E215">
-        <v>1.28277</v>
-      </c>
       <c r="F215">
         <v>1.28125</v>
       </c>
@@ -17565,18 +17049,6 @@
       <c r="A220" s="2">
         <v>43406</v>
       </c>
-      <c r="B220">
-        <v>1.29999</v>
-      </c>
-      <c r="C220">
-        <v>1.30407</v>
-      </c>
-      <c r="D220">
-        <v>1.29515</v>
-      </c>
-      <c r="E220">
-        <v>1.29661</v>
-      </c>
       <c r="F220">
         <v>1.29965</v>
       </c>
@@ -17950,18 +17422,6 @@
       <c r="A225" s="2">
         <v>43413</v>
       </c>
-      <c r="B225">
-        <v>1.30613</v>
-      </c>
-      <c r="C225">
-        <v>1.30701</v>
-      </c>
-      <c r="D225">
-        <v>1.29583</v>
-      </c>
-      <c r="E225">
-        <v>1.2974</v>
-      </c>
       <c r="F225">
         <v>1.30403</v>
       </c>
@@ -18341,18 +17801,6 @@
       <c r="A230" s="2">
         <v>43420</v>
       </c>
-      <c r="B230">
-        <v>1.27658</v>
-      </c>
-      <c r="C230">
-        <v>1.28774</v>
-      </c>
-      <c r="D230">
-        <v>1.27605</v>
-      </c>
-      <c r="E230">
-        <v>1.28208</v>
-      </c>
       <c r="F230">
         <v>1.28535</v>
       </c>
@@ -18726,18 +18174,6 @@
       <c r="A235" s="2">
         <v>43427</v>
       </c>
-      <c r="B235">
-        <v>1.28753</v>
-      </c>
-      <c r="C235">
-        <v>1.28827</v>
-      </c>
-      <c r="D235">
-        <v>1.27979</v>
-      </c>
-      <c r="E235">
-        <v>1.2808</v>
-      </c>
       <c r="F235">
         <v>1.28248</v>
       </c>
@@ -19111,18 +18547,6 @@
       <c r="A240" s="2">
         <v>43434</v>
       </c>
-      <c r="B240">
-        <v>1.27836</v>
-      </c>
-      <c r="C240">
-        <v>1.28095</v>
-      </c>
-      <c r="D240">
-        <v>1.2735</v>
-      </c>
-      <c r="E240">
-        <v>1.27488</v>
-      </c>
       <c r="F240">
         <v>1.2751</v>
       </c>
@@ -19508,18 +18932,6 @@
       <c r="A245" s="2">
         <v>43441</v>
       </c>
-      <c r="B245">
-        <v>1.27784</v>
-      </c>
-      <c r="C245">
-        <v>1.27901</v>
-      </c>
-      <c r="D245">
-        <v>1.27112</v>
-      </c>
-      <c r="E245">
-        <v>1.27319</v>
-      </c>
       <c r="F245">
         <v>1.27334</v>
       </c>
@@ -19899,18 +19311,6 @@
       <c r="A250" s="2">
         <v>43448</v>
       </c>
-      <c r="B250">
-        <v>1.26487</v>
-      </c>
-      <c r="C250">
-        <v>1.2663</v>
-      </c>
-      <c r="D250">
-        <v>1.25298</v>
-      </c>
-      <c r="E250">
-        <v>1.25839</v>
-      </c>
       <c r="F250">
         <v>1.25487</v>
       </c>
@@ -20284,18 +19684,6 @@
       <c r="A255" s="2">
         <v>43455</v>
       </c>
-      <c r="B255">
-        <v>1.26527</v>
-      </c>
-      <c r="C255">
-        <v>1.26978</v>
-      </c>
-      <c r="D255">
-        <v>1.26177</v>
-      </c>
-      <c r="E255">
-        <v>1.26254</v>
-      </c>
       <c r="F255">
         <v>1.26465</v>
       </c>
@@ -20361,18 +19749,6 @@
       <c r="A256" s="2">
         <v>43458</v>
       </c>
-      <c r="B256">
-        <v>1.26527</v>
-      </c>
-      <c r="C256">
-        <v>1.26978</v>
-      </c>
-      <c r="D256">
-        <v>1.26177</v>
-      </c>
-      <c r="E256">
-        <v>1.26254</v>
-      </c>
       <c r="F256">
         <v>1.27124</v>
       </c>
@@ -20598,18 +19974,6 @@
       <c r="A259" s="2">
         <v>43462</v>
       </c>
-      <c r="B259">
-        <v>1.26418</v>
-      </c>
-      <c r="C259">
-        <v>1.27076</v>
-      </c>
-      <c r="D259">
-        <v>1.26352</v>
-      </c>
-      <c r="E259">
-        <v>1.26959</v>
-      </c>
       <c r="F259">
         <v>1.26818</v>
       </c>
@@ -20674,18 +20038,6 @@
     <row r="260" spans="1:27">
       <c r="A260" s="2">
         <v>43465</v>
-      </c>
-      <c r="B260">
-        <v>1.26418</v>
-      </c>
-      <c r="C260">
-        <v>1.27076</v>
-      </c>
-      <c r="D260">
-        <v>1.26352</v>
-      </c>
-      <c r="E260">
-        <v>1.26959</v>
       </c>
       <c r="F260">
         <v>1.28061</v>

</xml_diff>